<commit_message>
[PHONGDV] Update meetting minus
</commit_message>
<xml_diff>
--- a/DOCS/Meetting_Minutes.xlsx
+++ b/DOCS/Meetting_Minutes.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 1_Date 12_5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -16,6 +16,56 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Action Item</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Coffee house ấp bắc</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>Identify Basic Requirement</t>
+  </si>
+  <si>
+    <t>Create excel sheet for basic story</t>
+  </si>
+  <si>
+    <t>Decide technical stack</t>
+  </si>
+  <si>
+    <t>all team member</t>
+  </si>
+  <si>
+    <t>create technical stack sheet</t>
+  </si>
+  <si>
+    <t>Raising github restructure</t>
+  </si>
+  <si>
+    <t>phong</t>
+  </si>
+  <si>
+    <t>restructure  git branch and permission</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +389,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43804.375</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>